<commit_message>
Updated Proteomics SVA & Matrisome Analysis
</commit_message>
<xml_diff>
--- a/Proteomics/Timecourse/analysis/02_gene-enrichment/output/GO_gsea_sva.xlsx
+++ b/Proteomics/Timecourse/analysis/02_gene-enrichment/output/GO_gsea_sva.xlsx
@@ -6,15 +6,16 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Diff_Treatment" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Terminal_vs_Baseline_Control" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Terminal_vs_Baseline_Metformin" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Diff_Disease" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Diff_Treatment" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Terminal_vs_Baseline_Control" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Terminal_vs_Baseline_Metformin" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -58,6 +59,54 @@
     <t xml:space="preserve">direction</t>
   </si>
   <si>
+    <t xml:space="preserve">GO:0007155</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cell adhesion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tags=58%, list=22%, signal=46%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENSECAG00000010267/ENSECAG00000020716/ENSECAG00000019596/ENSECAG00000016464/ENSECAG00000022498/ENSECAG00000020883/ENSECAG00000023141/ENSECAG00000014927/ENSECAG00000020488/ENSECAG00000020193/ENSECAG00000015369/ENSECAG00000008923/ENSECAG00000018584/ENSECAG00000001652/ENSECAG00000019665</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diff_Disease</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biological_process</t>
+  </si>
+  <si>
+    <t xml:space="preserve">down</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0005576</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extracellular region</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tags=54%, list=29%, signal=41%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENSECAG00000012362/ENSECAG00000020296/ENSECAG00000010239/ENSECAG00000022497/ENSECAG00000014858/ENSECAG00000008511/ENSECAG00000011321/ENSECAG00000012961/ENSECAG00000022279/ENSECAG00000055523/ENSECAG00000009896/ENSECAG00000007979/ENSECAG00000010481/ENSECAG00000057145/ENSECAG00000003355/ENSECAG00000013388/ENSECAG00000015294/ENSECAG00000016509/ENSECAG00000007865/ENSECAG00000019596/ENSECAG00000016475/ENSECAG00000012670/ENSECAG00000009752/ENSECAG00000004709/ENSECAG00000013324/ENSECAG00000011854/ENSECAG00000023141/ENSECAG00000016570/ENSECAG00000022165/ENSECAG00000010305/ENSECAG00000024697/ENSECAG00000018101/ENSECAG00000024138/ENSECAG00000000685/ENSECAG00000038712/ENSECAG00000015604/ENSECAG00000020413/ENSECAG00000015369/ENSECAG00000008923/ENSECAG00000018584/ENSECAG00000020769/ENSECAG00000011727/ENSECAG00000018178/ENSECAG00000015875/ENSECAG00000019665/ENSECAG00000010163/ENSECAG00000021011/ENSECAG00000007047/ENSECAG00000018717/ENSECAG00000017555/ENSECAG00000008859</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cellular_component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0005615</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extracellular space</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tags=50%, list=29%, signal=39%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENSECAG00000012362/ENSECAG00000020296/ENSECAG00000010239/ENSECAG00000022497/ENSECAG00000012064/ENSECAG00000006251/ENSECAG00000014858/ENSECAG00000011321/ENSECAG00000011574/ENSECAG00000017644/ENSECAG00000008303/ENSECAG00000022717/ENSECAG00000022279/ENSECAG00000009896/ENSECAG00000007979/ENSECAG00000010481/ENSECAG00000038107/ENSECAG00000018248/ENSECAG00000057145/ENSECAG00000015152/ENSECAG00000006474/ENSECAG00000000548/ENSECAG00000015294/ENSECAG00000016509/ENSECAG00000013764/ENSECAG00000007865/ENSECAG00000019596/ENSECAG00000010447/ENSECAG00000008270/ENSECAG00000016475/ENSECAG00000012670/ENSECAG00000009752/ENSECAG00000016570/ENSECAG00000014927/ENSECAG00000022165/ENSECAG00000010305/ENSECAG00000024697/ENSECAG00000018101/ENSECAG00000020881/ENSECAG00000024138/ENSECAG00000020193/ENSECAG00000038712/ENSECAG00000019069/ENSECAG00000015369/ENSECAG00000008923/ENSECAG00000024049/ENSECAG00000024967/ENSECAG00000010454/ENSECAG00000020769/ENSECAG00000006745/ENSECAG00000012506/ENSECAG00000011727/ENSECAG00000015875/ENSECAG00000019665/ENSECAG00000010163/ENSECAG00000021011/ENSECAG00000007047/ENSECAG00000017025/ENSECAG00000035543/ENSECAG00000017555</t>
+  </si>
+  <si>
     <t xml:space="preserve">GO:0010468</t>
   </si>
   <si>
@@ -67,28 +116,34 @@
     <t xml:space="preserve">tags=33%, list=3%, signal=33%</t>
   </si>
   <si>
-    <t xml:space="preserve">ENSECAG00000021929/ENSECAG00000012967/ENSECAG00000008577/ENSECAG00000008236</t>
+    <t xml:space="preserve">ENSECAG00000012967/ENSECAG00000021929/ENSECAG00000008577/ENSECAG00000008236</t>
   </si>
   <si>
     <t xml:space="preserve">Diff_Treatment</t>
   </si>
   <si>
-    <t xml:space="preserve">biological_process</t>
-  </si>
-  <si>
-    <t xml:space="preserve">down</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0060271</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cilium assembly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tags=54%, list=15%, signal=46%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENSECAG00000018714/ENSECAG00000023315/ENSECAG00000017216/ENSECAG00000028265/ENSECAG00000009219/ENSECAG00000013528/ENSECAG00000000300</t>
+    <t xml:space="preserve">GO:0005794</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Golgi apparatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tags=45%, list=17%, signal=39%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENSECAG00000045739/ENSECAG00000013307/ENSECAG00000009181/ENSECAG00000022694/ENSECAG00000010551/ENSECAG00000021818/ENSECAG00000041646/ENSECAG00000014460/ENSECAG00000022891/ENSECAG00000008742/ENSECAG00000008831/ENSECAG00000015099/ENSECAG00000013245/ENSECAG00000019125/ENSECAG00000009134/ENSECAG00000022341/ENSECAG00000012967/ENSECAG00000021929/ENSECAG00000008236/ENSECAG00000021359</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0030018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z disc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tags=46%, list=19%, signal=38%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENSECAG00000015514/ENSECAG00000012507/ENSECAG00000051991/ENSECAG00000024538/ENSECAG00000024273/ENSECAG00000009009/ENSECAG00000001034/ENSECAG00000021854/ENSECAG00000013832/ENSECAG00000019844/ENSECAG00000008577/ENSECAG00000011860</t>
   </si>
   <si>
     <t xml:space="preserve">GO:0007596</t>
@@ -97,61 +152,13 @@
     <t xml:space="preserve">blood coagulation</t>
   </si>
   <si>
-    <t xml:space="preserve">tags=62%, list=20%, signal=51%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENSECAG00000010239/ENSECAG00000008295/ENSECAG00000000527/ENSECAG00000008280/ENSECAG00000027768/ENSECAG00000000283/ENSECAG00000013924/ENSECAG00000015294/ENSECAG00000024697/ENSECAG00000016570</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0030018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z disc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tags=38%, list=15%, signal=33%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENSECAG00000012507/ENSECAG00000009009/ENSECAG00000024538/ENSECAG00000024273/ENSECAG00000001034/ENSECAG00000021854/ENSECAG00000013832/ENSECAG00000008577/ENSECAG00000019844/ENSECAG00000011860</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cellular_component</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0005794</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Golgi apparatus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tags=36%, list=13%, signal=33%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENSECAG00000009181/ENSECAG00000045739/ENSECAG00000008742/ENSECAG00000008831/ENSECAG00000010551/ENSECAG00000041646/ENSECAG00000009134/ENSECAG00000015099/ENSECAG00000014460/ENSECAG00000013245/ENSECAG00000019125/ENSECAG00000022341/ENSECAG00000021929/ENSECAG00000012967/ENSECAG00000008236/ENSECAG00000021359</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0010008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">endosome membrane</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tags=40%, list=10%, signal=36%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENSECAG00000017216/ENSECAG00000028265/ENSECAG00000026807/ENSECAG00000010711/ENSECAG00000017473/ENSECAG00000017618</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0043025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">neuronal cell body</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tags=75%, list=27%, signal=55%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENSECAG00000018948/ENSECAG00000008958/ENSECAG00000018670/ENSECAG00000008511/ENSECAG00000018626/ENSECAG00000024827/ENSECAG00000005572/ENSECAG00000007386/ENSECAG00000013252/ENSECAG00000021914/ENSECAG00000012967/ENSECAG00000015766</t>
+    <t xml:space="preserve">tags=50%, list=15%, signal=43%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENSECAG00000010239/ENSECAG00000008280/ENSECAG00000024697/ENSECAG00000011321/ENSECAG00000027768/ENSECAG00000000283/ENSECAG00000015294/ENSECAG00000000527</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terminal_vs_Baseline_Control</t>
   </si>
   <si>
     <t xml:space="preserve">GO:0007420</t>
@@ -163,64 +170,25 @@
     <t xml:space="preserve">tags=40%, list=5%, signal=38%</t>
   </si>
   <si>
-    <t xml:space="preserve">ENSECAG00000021359/ENSECAG00000012360/ENSECAG00000011846/ENSECAG00000024560</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Terminal_vs_Baseline_Control</t>
+    <t xml:space="preserve">ENSECAG00000012360/ENSECAG00000021359/ENSECAG00000024560/ENSECAG00000011846</t>
   </si>
   <si>
     <t xml:space="preserve">up</t>
   </si>
   <si>
-    <t xml:space="preserve">tags=62%, list=12%, signal=56%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENSECAG00000014646/ENSECAG00000007979/ENSECAG00000010239/ENSECAG00000008280/ENSECAG00000024697/ENSECAG00000011321/ENSECAG00000027768/ENSECAG00000000283/ENSECAG00000015294/ENSECAG00000000527</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tags=56%, list=13%, signal=49%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENSECAG00000007979/ENSECAG00000010239/ENSECAG00000011321/ENSECAG00000008280/ENSECAG00000024697/ENSECAG00000027768/ENSECAG00000000283/ENSECAG00000015294/ENSECAG00000000527</t>
+    <t xml:space="preserve">tags=45%, list=20%, signal=38%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENSECAG00000008236/ENSECAG00000021359/ENSECAG00000009134/ENSECAG00000012967/ENSECAG00000041646/ENSECAG00000014460/ENSECAG00000019125/ENSECAG00000014846/ENSECAG00000019611/ENSECAG00000013245/ENSECAG00000022694/ENSECAG00000055523/ENSECAG00000008742/ENSECAG00000021929/ENSECAG00000013307/ENSECAG00000014858/ENSECAG00000012506/ENSECAG00000022341/ENSECAG00000051009/ENSECAG00000008831</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tags=50%, list=10%, signal=46%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENSECAG00000011321/ENSECAG00000010239/ENSECAG00000008280/ENSECAG00000024697/ENSECAG00000027768/ENSECAG00000000283/ENSECAG00000015294/ENSECAG00000000527</t>
   </si>
   <si>
     <t xml:space="preserve">Terminal_vs_Baseline_Metformin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0007599</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hemostasis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tags=64%, list=13%, signal=56%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENSECAG00000007979/ENSECAG00000010239/ENSECAG00000011321/ENSECAG00000008280/ENSECAG00000024697/ENSECAG00000027768/ENSECAG00000015294</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0005884</t>
-  </si>
-  <si>
-    <t xml:space="preserve">actin filament</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tags=50%, list=11%, signal=45%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENSECAG00000015460/ENSECAG00000019476/ENSECAG00000015935/ENSECAG00000024788/ENSECAG00000004482/ENSECAG00000000207/ENSECAG00000013528</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0005576</t>
-  </si>
-  <si>
-    <t xml:space="preserve">extracellular region</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tags=32%, list=14%, signal=30%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENSECAG00000020769/ENSECAG00000018101/ENSECAG00000007979/ENSECAG00000020296/ENSECAG00000017637/ENSECAG00000016509/ENSECAG00000003355/ENSECAG00000010239/ENSECAG00000011321/ENSECAG00000013968/ENSECAG00000008365/ENSECAG00000024138/ENSECAG00000000701/ENSECAG00000018717/ENSECAG00000015875/ENSECAG00000024792/ENSECAG00000011727/ENSECAG00000008280/ENSECAG00000018178/ENSECAG00000007010/ENSECAG00000002111/ENSECAG00000024697/ENSECAG00000022165/ENSECAG00000012558/ENSECAG00000027768/ENSECAG00000025159/ENSECAG00000019868/ENSECAG00000015294/ENSECAG00000008923/ENSECAG00000015766</t>
   </si>
 </sst>
 </file>
@@ -268,8 +236,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:N8" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:N8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:N4" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:N4"/>
   <tableColumns count="14">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="Description"/>
@@ -291,8 +259,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:N3" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:N3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:N4" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:N4"/>
   <tableColumns count="14">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="Description"/>
@@ -314,8 +282,31 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:N5" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:N5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:N4" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:N4"/>
+  <tableColumns count="14">
+    <tableColumn id="1" name="ID"/>
+    <tableColumn id="2" name="Description"/>
+    <tableColumn id="3" name="setSize"/>
+    <tableColumn id="4" name="enrichmentScore"/>
+    <tableColumn id="5" name="NES"/>
+    <tableColumn id="6" name="pvalue"/>
+    <tableColumn id="7" name="p.adjust"/>
+    <tableColumn id="8" name="qvalue"/>
+    <tableColumn id="9" name="rank"/>
+    <tableColumn id="10" name="leading_edge"/>
+    <tableColumn id="11" name="core_enrichment"/>
+    <tableColumn id="12" name="Contrast"/>
+    <tableColumn id="13" name="Database"/>
+    <tableColumn id="14" name="direction"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:N2" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:N2"/>
   <tableColumns count="14">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="Description"/>
@@ -673,25 +664,25 @@
         <v>15</v>
       </c>
       <c r="C2" t="n">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.772334908541806</v>
+        <v>-0.5993380961369</v>
       </c>
       <c r="E2" t="n">
-        <v>-1.87250339079297</v>
+        <v>-1.93708373807688</v>
       </c>
       <c r="F2" t="n">
-        <v>0.000463690527719418</v>
+        <v>0.000870080060153242</v>
       </c>
       <c r="G2" t="n">
-        <v>0.045441671716503</v>
+        <v>0.0852678458950177</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0434404810179244</v>
+        <v>0.0815127635301459</v>
       </c>
       <c r="I2" t="n">
-        <v>38</v>
+        <v>266</v>
       </c>
       <c r="J2" t="s">
         <v>16</v>
@@ -717,25 +708,25 @@
         <v>22</v>
       </c>
       <c r="C3" t="n">
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.727670129671746</v>
+        <v>-0.475210821483986</v>
       </c>
       <c r="E3" t="n">
-        <v>-1.81027933019977</v>
+        <v>-2.04866292012275</v>
       </c>
       <c r="F3" t="n">
-        <v>0.00139838330577432</v>
+        <v>0.00000773528317816837</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0685207819829418</v>
+        <v>0.000750322468282332</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0655032180073235</v>
+        <v>0.000683961881016993</v>
       </c>
       <c r="I3" t="n">
-        <v>199</v>
+        <v>361</v>
       </c>
       <c r="J3" t="s">
         <v>23</v>
@@ -747,7 +738,7 @@
         <v>18</v>
       </c>
       <c r="M3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="N3" t="s">
         <v>20</v>
@@ -755,221 +746,45 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C4" t="n">
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.668117517318781</v>
+        <v>-0.431886933171487</v>
       </c>
       <c r="E4" t="n">
-        <v>-1.7345223160483</v>
+        <v>-1.93971087064703</v>
       </c>
       <c r="F4" t="n">
-        <v>0.00297636744860384</v>
+        <v>0.0000167059736380492</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0972280033210587</v>
+        <v>0.000810239721445384</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0929462115528918</v>
+        <v>0.000738579887155857</v>
       </c>
       <c r="I4" t="n">
-        <v>263</v>
+        <v>361</v>
       </c>
       <c r="J4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L4" t="s">
         <v>18</v>
       </c>
       <c r="M4" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="N4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" t="n">
-        <v>26</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-0.665324680007531</v>
-      </c>
-      <c r="E5" t="n">
-        <v>-1.96601438742162</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.00025723896082006</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.0249521791995458</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.0222037839865736</v>
-      </c>
-      <c r="I5" t="n">
-        <v>197</v>
-      </c>
-      <c r="J5" t="s">
-        <v>31</v>
-      </c>
-      <c r="K5" t="s">
-        <v>32</v>
-      </c>
-      <c r="L5" t="s">
-        <v>18</v>
-      </c>
-      <c r="M5" t="s">
-        <v>33</v>
-      </c>
-      <c r="N5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" t="n">
-        <v>44</v>
-      </c>
-      <c r="D6" t="n">
-        <v>-0.554316948152268</v>
-      </c>
-      <c r="E6" t="n">
-        <v>-1.8099599166791</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.00125506437253244</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.0608706220678235</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.054165936077716</v>
-      </c>
-      <c r="I6" t="n">
-        <v>173</v>
-      </c>
-      <c r="J6" t="s">
-        <v>36</v>
-      </c>
-      <c r="K6" t="s">
-        <v>37</v>
-      </c>
-      <c r="L6" t="s">
-        <v>18</v>
-      </c>
-      <c r="M6" t="s">
-        <v>33</v>
-      </c>
-      <c r="N6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" t="n">
-        <v>15</v>
-      </c>
-      <c r="D7" t="n">
-        <v>-0.700305278920779</v>
-      </c>
-      <c r="E7" t="n">
-        <v>-1.82429123892326</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.00248882730515975</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.080472082866832</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.0716083645695087</v>
-      </c>
-      <c r="I7" t="n">
-        <v>133</v>
-      </c>
-      <c r="J7" t="s">
-        <v>40</v>
-      </c>
-      <c r="K7" t="s">
-        <v>41</v>
-      </c>
-      <c r="L7" t="s">
-        <v>18</v>
-      </c>
-      <c r="M7" t="s">
-        <v>33</v>
-      </c>
-      <c r="N7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" t="n">
-        <v>16</v>
-      </c>
-      <c r="D8" t="n">
-        <v>-0.675409521482415</v>
-      </c>
-      <c r="E8" t="n">
-        <v>-1.79837083779305</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.00364232233939954</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.0883263167304389</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.078597482060727</v>
-      </c>
-      <c r="I8" t="n">
-        <v>358</v>
-      </c>
-      <c r="J8" t="s">
-        <v>44</v>
-      </c>
-      <c r="K8" t="s">
-        <v>45</v>
-      </c>
-      <c r="L8" t="s">
-        <v>18</v>
-      </c>
-      <c r="M8" t="s">
-        <v>33</v>
-      </c>
-      <c r="N8" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1036,89 +851,133 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="C2" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D2" t="n">
-        <v>0.787437898329961</v>
+        <v>-0.806979185695809</v>
       </c>
       <c r="E2" t="n">
-        <v>1.91002951800082</v>
+        <v>-1.92840211821899</v>
       </c>
       <c r="F2" t="n">
-        <v>0.000629654895226098</v>
+        <v>0.000247486474324637</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0617061797321576</v>
+        <v>0.0242536744838144</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0596515163898409</v>
+        <v>0.0229250628848085</v>
       </c>
       <c r="I2" t="n">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="J2" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="K2" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="L2" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="M2" t="s">
         <v>19</v>
       </c>
       <c r="N2" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="n">
+        <v>44</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-0.59088923010819</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-1.88782332249324</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.0000901202166048704</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.00874166101067243</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.00796852441558854</v>
+      </c>
+      <c r="I3" t="n">
+        <v>211</v>
+      </c>
+      <c r="J3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" t="s">
+      <c r="N3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" t="n">
         <v>26</v>
       </c>
-      <c r="C3" t="n">
-        <v>16</v>
-      </c>
-      <c r="D3" t="n">
-        <v>-0.697319388900172</v>
-      </c>
-      <c r="E3" t="n">
-        <v>-1.85257277531727</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.0016254725888367</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.0796481568529984</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.076996069997528</v>
-      </c>
-      <c r="I3" t="n">
-        <v>159</v>
-      </c>
-      <c r="J3" t="s">
-        <v>52</v>
-      </c>
-      <c r="K3" t="s">
-        <v>53</v>
-      </c>
-      <c r="L3" t="s">
-        <v>50</v>
-      </c>
-      <c r="M3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N3" t="s">
+      <c r="D4" t="n">
+        <v>-0.632916701508686</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-1.81164571292053</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.00181910698496479</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.0882266887707922</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.0804236772300222</v>
+      </c>
+      <c r="I4" t="n">
+        <v>228</v>
+      </c>
+      <c r="J4" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1185,40 +1044,40 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C2" t="n">
         <v>16</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.792544498410989</v>
+        <v>-0.706918639372572</v>
       </c>
       <c r="E2" t="n">
-        <v>-2.04933290956824</v>
+        <v>-1.90337359097825</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0000727231645397612</v>
+        <v>0.00148547508600348</v>
       </c>
       <c r="G2" t="n">
-        <v>0.00712687012489659</v>
+        <v>0.0727882792141705</v>
       </c>
       <c r="H2" t="n">
-        <v>0.00711921505494504</v>
+        <v>0.0703646093370069</v>
       </c>
       <c r="I2" t="n">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="J2" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="K2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="L2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="M2" t="s">
         <v>19</v>
@@ -1229,134 +1088,90 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C3" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.798379776007797</v>
+        <v>0.765973082736173</v>
       </c>
       <c r="E3" t="n">
-        <v>-1.86208023277952</v>
+        <v>1.83100824234886</v>
       </c>
       <c r="F3" t="n">
-        <v>0.00129459707439274</v>
+        <v>0.000950697904023176</v>
       </c>
       <c r="G3" t="n">
-        <v>0.063435256645244</v>
+        <v>0.0727882792141705</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0633671199571181</v>
+        <v>0.0703646093370069</v>
       </c>
       <c r="I3" t="n">
-        <v>173</v>
+        <v>66</v>
       </c>
       <c r="J3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="K3" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="L3" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="M3" t="s">
         <v>19</v>
       </c>
       <c r="N3" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="C4" t="n">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.762611331780968</v>
+        <v>0.514582042852168</v>
       </c>
       <c r="E4" t="n">
-        <v>-1.90722117451544</v>
+        <v>1.81922571827569</v>
       </c>
       <c r="F4" t="n">
-        <v>0.000462263588191706</v>
+        <v>0.000794883909538921</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0448395680545955</v>
+        <v>0.0771037392252754</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0418470195626176</v>
+        <v>0.0686110321917806</v>
       </c>
       <c r="I4" t="n">
-        <v>140</v>
+        <v>243</v>
       </c>
       <c r="J4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="K4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="L4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="M4" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="N4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" t="n">
-        <v>94</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-0.468333479455654</v>
-      </c>
-      <c r="E5" t="n">
-        <v>-1.6690805737971</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.00116354147950934</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.0564317617562032</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.0526655617041072</v>
-      </c>
-      <c r="I5" t="n">
-        <v>177</v>
-      </c>
-      <c r="J5" t="s">
-        <v>67</v>
-      </c>
-      <c r="K5" t="s">
-        <v>68</v>
-      </c>
-      <c r="L5" t="s">
-        <v>56</v>
-      </c>
-      <c r="M5" t="s">
-        <v>33</v>
-      </c>
-      <c r="N5" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1366,4 +1181,109 @@
     <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="n">
+        <v>16</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-0.812042986595372</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-2.07944272363881</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.0000327902466030113</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.00321344416709511</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.00320999256218953</v>
+      </c>
+      <c r="I2" t="n">
+        <v>122</v>
+      </c>
+      <c r="J2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K2" t="s">
+        <v>56</v>
+      </c>
+      <c r="L2" t="s">
+        <v>57</v>
+      </c>
+      <c r="M2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId6"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>